<commit_message>
core game mechanics finished, inital manager tests
</commit_message>
<xml_diff>
--- a/DevLog/DevLog.xlsx
+++ b/DevLog/DevLog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Game Building\CurrentProjects\DogWalkingGame\DevLog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB0E993-A8E2-412E-A3D3-F3F27132390F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38300D33-80C8-4054-B606-29CC967DEA67}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10452" yWindow="4656" windowWidth="25560" windowHeight="15276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -48,10 +48,16 @@
     <t>Rope minikit from asset store will work for this game's purpose.</t>
   </si>
   <si>
-    <t>"Player.cs" Unit Tests</t>
-  </si>
-  <si>
-    <t>Package Rope Physics Exploration/"Player.cs" Unit Tests</t>
+    <t>Package Rope Physics Exploration/Player Unit Tests</t>
+  </si>
+  <si>
+    <t>Player Unit Tests</t>
+  </si>
+  <si>
+    <t>Dog Unit Tests</t>
+  </si>
+  <si>
+    <t>SpawnManager/Obstacle/GameManager Unit Tests</t>
   </si>
 </sst>
 </file>
@@ -379,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -426,7 +432,7 @@
         <v>44257</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <v>4</v>
@@ -440,10 +446,65 @@
         <v>44258</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>44259</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>44260</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
         <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>44261</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>44262</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>44263</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>